<commit_message>
turns out editing still didn't work
</commit_message>
<xml_diff>
--- a/2500.xlsx
+++ b/2500.xlsx
@@ -18885,7 +18885,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19174,7 +19174,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19344,7 +19344,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes and word updates
</commit_message>
<xml_diff>
--- a/2500.xlsx
+++ b/2500.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="12" activeTab="27" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="12" activeTab="30" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="2500" sheetId="1" state="visible" r:id="rId1"/>
@@ -17808,7 +17808,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -17825,7 +17825,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -17859,7 +17859,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -17876,7 +17876,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -17995,7 +17995,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18012,7 +18012,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18046,7 +18046,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18080,7 +18080,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18131,7 +18131,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18165,7 +18165,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18267,7 +18267,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18352,7 +18352,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18403,7 +18403,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18437,7 +18437,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18454,7 +18454,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18556,7 +18556,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18573,7 +18573,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18607,7 +18607,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18698,7 +18698,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18715,7 +18715,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18749,7 +18749,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18817,7 +18817,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18834,7 +18834,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18919,7 +18919,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18936,7 +18936,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18953,7 +18953,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -18970,7 +18970,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19004,7 +19004,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19038,7 +19038,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19106,7 +19106,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19123,7 +19123,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19140,7 +19140,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19157,7 +19157,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19191,7 +19191,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19208,7 +19208,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19259,7 +19259,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19293,7 +19293,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19310,7 +19310,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19327,7 +19327,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19361,7 +19361,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19412,7 +19412,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19429,7 +19429,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19446,7 +19446,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19463,7 +19463,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19514,7 +19514,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -19531,7 +19531,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>wrong</t>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -21539,7 +21539,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21558,6 +21558,11 @@
           <t>een verzekering</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -21570,6 +21575,11 @@
           <t>een bar</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -21582,6 +21592,11 @@
           <t>een praktijk, een cabinet</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -21594,6 +21609,11 @@
           <t>zeker</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -21606,6 +21626,11 @@
           <t>de jacht</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -21618,6 +21643,11 @@
           <t>een burger</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -21630,6 +21660,11 @@
           <t>commercieel</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -21642,6 +21677,11 @@
           <t>een mededeling</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -21654,6 +21694,11 @@
           <t>de communicatie</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -21666,6 +21711,11 @@
           <t>de bouw, de aanleg</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -21678,6 +21728,11 @@
           <t>een gang, een rijstrook</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -21690,6 +21745,11 @@
           <t>sterven</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -21702,6 +21762,11 @@
           <t>een verklaring, een aangifte</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -21714,6 +21779,11 @@
           <t>aanwijzen</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -21726,6 +21796,11 @@
           <t>verlangen naar, sterk willen</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -21738,6 +21813,11 @@
           <t>een lot</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -21750,6 +21830,11 @@
           <t>een uitwisseling</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -21762,6 +21847,11 @@
           <t>een hel</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -21774,6 +21864,11 @@
           <t>de verveling</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -21786,6 +21881,11 @@
           <t>een probleem</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -21798,6 +21898,11 @@
           <t>een fase, een stap, een rit</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -21810,6 +21915,11 @@
           <t>enz.</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -21822,6 +21932,11 @@
           <t>de financiën</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -21834,6 +21949,11 @@
           <t>een vrucht, fruit</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -21846,6 +21966,11 @@
           <t>geweldig, geniaal</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -21858,6 +21983,11 @@
           <t>het beheer</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -21870,6 +22000,11 @@
           <t>de hoogte</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -21882,6 +22017,11 @@
           <t>een flatgebouw</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -21894,6 +22034,11 @@
           <t>inspireren</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -21906,6 +22051,11 @@
           <t>inspiratie halen uit</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -21918,6 +22068,11 @@
           <t>een investering</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -21930,6 +22085,11 @@
           <t>wassen</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -21942,6 +22102,11 @@
           <t>zich wassen</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -21954,6 +22119,11 @@
           <t>ziek</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -21966,6 +22136,11 @@
           <t>prachtig, schitterend</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -21978,6 +22153,11 @@
           <t>een mijn, een voorkomen</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -21990,6 +22170,11 @@
           <t>een munt</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -22002,6 +22187,11 @@
           <t>het kleingeld</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -22014,6 +22204,11 @@
           <t>overleden</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -22026,6 +22221,11 @@
           <t>een motor</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -22038,6 +22238,11 @@
           <t>een geboorte</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -22050,6 +22255,11 @@
           <t>duidelijk, netto</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -22062,6 +22272,11 @@
           <t>wegen</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -22074,6 +22289,11 @@
           <t>een politieagent</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -22086,6 +22306,11 @@
           <t>het voorjaar</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -22098,6 +22323,11 @@
           <t>ontzeggen, ontnemen</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -22110,6 +22340,11 @@
           <t>zich ontzeggen</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -22122,6 +22357,11 @@
           <t>waarschijnlijk</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -22134,6 +22374,11 @@
           <t>wegsturen, terugsturen, weerkaatsen</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -22146,6 +22391,11 @@
           <t>begroeten, toejuichen</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -22158,6 +22408,11 @@
           <t>elkaar begroeten</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -22170,6 +22425,11 @@
           <t>schudden</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -22182,6 +22442,11 @@
           <t>geheim</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -22194,6 +22459,11 @@
           <t>een top, een topontmoeting</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -22206,6 +22476,11 @@
           <t>denken aan</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -22218,6 +22493,11 @@
           <t>een stijl</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -22228,6 +22508,11 @@
       <c r="B57" t="inlineStr">
         <is>
           <t>het transport</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -22242,7 +22527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22261,6 +22546,11 @@
           <t>verliefd</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -22273,6 +22563,11 @@
           <t>een apparaat</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -22285,6 +22580,11 @@
           <t>een verwachting, het wachten</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -22297,6 +22597,11 @@
           <t>een voordeel</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -22309,6 +22614,11 @@
           <t>breken, verbreken, verbrijzelen</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -22321,6 +22631,11 @@
           <t>breken</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -22333,6 +22648,11 @@
           <t>een schoen</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -22345,6 +22665,11 @@
           <t>een sterke daling, een val</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -22357,6 +22682,11 @@
           <t>vijftig</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -22369,6 +22699,11 @@
           <t>volledig, compleet</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -22381,6 +22716,11 @@
           <t>samenstellen</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -22393,6 +22733,11 @@
           <t>bestaan uit</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -22405,6 +22750,11 @@
           <t>bevatten</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -22417,6 +22767,11 @@
           <t>tevredenstellen</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -22429,6 +22784,11 @@
           <t>zich tevredenstellen met</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -22441,6 +22801,11 @@
           <t>een dans</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -22453,6 +22818,11 @@
           <t>afhangen van</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -22465,6 +22835,11 @@
           <t>een discussie</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -22477,6 +22852,11 @@
           <t>een bepaling, een regeling</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -22489,6 +22869,11 @@
           <t>een afstand</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -22501,6 +22886,11 @@
           <t>opsluiten</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -22513,6 +22903,11 @@
           <t>zich opsluiten</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -22525,6 +22920,11 @@
           <t>opnemen, optekenen</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -22537,6 +22937,11 @@
           <t>zich registreren, inchecken</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -22549,6 +22954,11 @@
           <t>uitzetten</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -22561,6 +22971,11 @@
           <t>uitdoven, sterven</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -22573,6 +22988,11 @@
           <t>exact</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -22585,6 +23005,11 @@
           <t>extreem</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -22597,6 +23022,11 @@
           <t>een finale</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -22609,6 +23039,11 @@
           <t>een krankzinnige</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -22621,6 +23056,11 @@
           <t>de kou</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -22633,6 +23073,11 @@
           <t>onmiddelijk</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -22645,6 +23090,11 @@
           <t>een grens, een limiet</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -22657,6 +23107,11 @@
           <t>de beste</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -22669,6 +23124,11 @@
           <t>een aanbod, een bod</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -22681,6 +23141,11 @@
           <t>een pakket</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -22693,6 +23158,11 @@
           <t>een schilderij</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -22705,6 +23175,11 @@
           <t>slechter</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -22717,6 +23192,11 @@
           <t>[uit]persen, [aan]dringen</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -22729,6 +23209,11 @@
           <t>beweren, doen alsof</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -22741,6 +23226,11 @@
           <t>wandelen</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -22753,6 +23243,11 @@
           <t>krachtig, machtig</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -22765,16 +23260,26 @@
           <t>verzamelen, samenbrengen</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>se rasssembler</t>
+          <t>se rassembler</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
           <t>bijeenkomen</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -22789,6 +23294,11 @@
           <t>achteruitgaan</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -22801,16 +23311,26 @@
           <t>weer ophalen, terugwinnen</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>un répas</t>
+          <t>un repas</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>een maaltijd</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -22825,6 +23345,11 @@
           <t>het zand</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -22837,6 +23362,11 @@
           <t>een adem</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -22849,6 +23379,11 @@
           <t>voorleggen, onderwerpen [aan]</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -22861,6 +23396,11 @@
           <t>zich onderwerpen aan</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -22873,6 +23413,11 @@
           <t>een thema, een onderwerp</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -22885,6 +23430,11 @@
           <t>het onrecht, het ongelijk</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -22897,6 +23447,11 @@
           <t>vertalen</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -22909,6 +23464,11 @@
           <t>vertaald worden</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -22921,6 +23481,11 @@
           <t>een streep, een kenmerk, een eigenschap</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -22933,6 +23498,11 @@
           <t>een wereld</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -22945,6 +23515,11 @@
           <t>het universum</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -22957,6 +23532,11 @@
           <t>gieten, storten</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -22967,6 +23547,11 @@
       <c r="B60" t="inlineStr">
         <is>
           <t>stemmen</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>correct</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new /diff tag, progress bar now scales correctly
</commit_message>
<xml_diff>
--- a/2500.xlsx
+++ b/2500.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="12" activeTab="30" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="12" activeTab="13" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="2500" sheetId="1" state="visible" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="4.4" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="4.5" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="4.6" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="4.7" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -466,7 +467,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="14.109375" bestFit="1" customWidth="1" min="1" max="3"/>
   </cols>
@@ -1423,7 +1424,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="14.109375" bestFit="1" customWidth="1" min="1" max="3"/>
   </cols>
@@ -10711,7 +10712,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="34.88671875" customWidth="1" min="1" max="1"/>
     <col width="33.77734375" customWidth="1" min="2" max="2"/>
@@ -12709,7 +12710,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="27.6640625" customWidth="1" min="1" max="1"/>
     <col width="37" customWidth="1" min="2" max="2"/>
@@ -15813,7 +15814,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="47.77734375" customWidth="1" min="1" max="1"/>
     <col width="36.6640625" customWidth="1" min="2" max="2"/>
@@ -18645,7 +18646,7 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="46.109375" customWidth="1" min="2" max="2"/>
@@ -23560,6 +23561,926 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>une amitié</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>een vriendschap</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>autrefois</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>voorheen, vroeger</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>une bière</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>een bier</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>blond</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>blond</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>calme</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>kalm, rustig</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>un camion</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>een vrachtwagen</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>une cellule</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>een cel</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>chasser</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>jagen [op], verjagen</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>une chemise</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>een hemd, een overhemd</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>un, une commissaire</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>een commissaris</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>se dépêcher</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>zich haasten</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>dirigeant</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>leidinggevend, leidend</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>un disque</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>een schijf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>un dommage</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>een schade</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>une émission</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>een programma, een uitzending</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>une énergie</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>een energie</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>enforcer</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>indrukken, intrappen</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>s'enforcer dans</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>wegzinken in, wegzakken in</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>un entraineur</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>een trainer</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>un entretien</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>een onderhoud, een interview</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>un établissement</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>een instelling</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>examiner</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>onderzoeken</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>une fédération</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>een federatie</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ferme</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>stevig</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>un gardien</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>een bewaker</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>gêner</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>storen, verstoren, in verlegenheid brengen</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>se gêner</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>zich schamen, elkaar in de weg lopen</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>une grève</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>een staking</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>incroyable</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ongeloofelijk, geweldig</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>une instruction</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>een opdracht, een instructie</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>judiciaire</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>gerechtelijk</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>un lieutenant</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>een luitenant</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>une manifestation</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>een betoging</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>une menace</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>een bedreiging</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>la neige</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>de sneeuw</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>parfait</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>perfect</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>un particulier</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>een particulier, een individu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>un, une pauvre</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>een arme</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>une pomme</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>een appel</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>un portrait</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>een portret</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>une pratique</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>een gebruik</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>un rang</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>een rang</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ranger</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>opruimen</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>la retraite</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>het pensioen, het terugtrekken</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>un rythme</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>een ritme</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>une séance</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>een zitting</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>le secours</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>de hulp</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>un talent</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>een talent</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>téléphoner [à]</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>telefoneren [naar]</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>se téléphoner</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>elkaar opbellen</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>totaal</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>une urgence</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>een noodsituatie</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>vaste</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>uitgebreid, ruim</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>